<commit_message>
avancer le code pour ecrire dans l'excel
</commit_message>
<xml_diff>
--- a/SAE_3_01/S2.xlsx
+++ b/SAE_3_01/S2.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="B2" s="28" t="inlineStr">
         <is>
-          <t>R1.01 Initiation au développement</t>
+          <t>R1.07</t>
         </is>
       </c>
       <c r="E2" s="28" t="n"/>
@@ -780,7 +780,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -854,13 +854,13 @@
     <row r="5">
       <c r="A5" s="28" t="n"/>
       <c r="B5" s="28" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C5" s="28" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D5" s="28" t="n">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E5" s="28" t="n"/>
       <c r="F5" s="28" t="n"/>

</xml_diff>